<commit_message>
改老的reg + prov analysis
</commit_message>
<xml_diff>
--- a/Data/CN_Policy-不用了/各省一级响应.xlsx
+++ b/Data/CN_Policy-不用了/各省一级响应.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qitianhu/Documents/Research/Explore/COVID-19_sosc/CN_Provinces/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qitianhu/Documents/Research/Explore/COVID-19_sosc/Data/CN_Policy-不用了/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B51A2D5-9121-F643-85E6-19F16BD7DBC6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75977858-7CC3-8844-8413-A3DD7A241F59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="21940" windowWidth="27540" windowHeight="17040" xr2:uid="{ACB78A26-02EA-2D41-B8F7-6F6A16A4587F}"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="17540" xr2:uid="{ACB78A26-02EA-2D41-B8F7-6F6A16A4587F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>prov</t>
   </si>
@@ -127,6 +127,102 @@
   </si>
   <si>
     <t>erji_date</t>
+  </si>
+  <si>
+    <t>安徽省</t>
+  </si>
+  <si>
+    <t>云南省</t>
+  </si>
+  <si>
+    <t>湖南省</t>
+  </si>
+  <si>
+    <t>广西壮族自治区</t>
+  </si>
+  <si>
+    <t>河北省</t>
+  </si>
+  <si>
+    <t>陕西省</t>
+  </si>
+  <si>
+    <t>青海省</t>
+  </si>
+  <si>
+    <t>湖北省</t>
+  </si>
+  <si>
+    <t>甘肃省</t>
+  </si>
+  <si>
+    <t>新疆维吾尔自治区</t>
+  </si>
+  <si>
+    <t>辽宁省</t>
+  </si>
+  <si>
+    <t>吉林省</t>
+  </si>
+  <si>
+    <t>河南省</t>
+  </si>
+  <si>
+    <t>四川省</t>
+  </si>
+  <si>
+    <t>江西省</t>
+  </si>
+  <si>
+    <t>贵州省</t>
+  </si>
+  <si>
+    <t>山西省</t>
+  </si>
+  <si>
+    <t>内蒙古自治区</t>
+  </si>
+  <si>
+    <t>黑龙江省</t>
+  </si>
+  <si>
+    <t>广东省</t>
+  </si>
+  <si>
+    <t>福建省</t>
+  </si>
+  <si>
+    <t>西藏自治区</t>
+  </si>
+  <si>
+    <t>海南省</t>
+  </si>
+  <si>
+    <t>浙江省</t>
+  </si>
+  <si>
+    <t>宁夏回族自治区</t>
+  </si>
+  <si>
+    <t>江苏省</t>
+  </si>
+  <si>
+    <t>山东省</t>
+  </si>
+  <si>
+    <t>天津市</t>
+  </si>
+  <si>
+    <t>北京市</t>
+  </si>
+  <si>
+    <t>上海市</t>
+  </si>
+  <si>
+    <t>重庆市</t>
+  </si>
+  <si>
+    <t>prov_full</t>
   </si>
 </sst>
 </file>
@@ -162,9 +258,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,15 +576,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA467B8-5F20-8E47-AE81-F6DBED386C91}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,32 +594,44 @@
       <c r="C1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>43853</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>43853</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>43853</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -532,221 +641,306 @@
       <c r="C5" s="1">
         <v>43852</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="1">
         <v>43855</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="1">
         <v>43856</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="1">
         <v>43857</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>